<commit_message>
exporting scripted test cases
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/import-columns.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/import-columns.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace_squashtm\squashtest-tm-staging\tm\tm.service\src\test\resources\batchimport\testcase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987"/>
   </bookViews>
   <sheets>
-    <sheet name="TEST_CASES" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="STEPS" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="PARAMETERS" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="DATASETS" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="TEST_CASES" sheetId="1" r:id="rId1"/>
+    <sheet name="STEPS" sheetId="2" r:id="rId2"/>
+    <sheet name="PARAMETERS" sheetId="3" r:id="rId3"/>
+    <sheet name="DATASETS" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="155">
   <si>
     <t>ACTION</t>
   </si>
@@ -474,17 +478,22 @@
   </si>
   <si>
     <t>param/owner/path/8</t>
+  </si>
+  <si>
+    <t>TC_KIND</t>
+  </si>
+  <si>
+    <t>TC_SCRIPTING_LANGUAGE</t>
+  </si>
+  <si>
+    <t>TC_SCRIPT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -493,22 +502,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -525,186 +519,471 @@
     </fill>
   </fills>
   <borders count="7">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AB9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB2" activeCellId="0" sqref="AB2"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.56632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.56632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.00510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0051020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.5765306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.4234693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.2857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.1428571428571"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.2857142857143"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.29081632653061"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.7091836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.8571428571429"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.5765306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.70918367346939"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.8571428571429"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.4234693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.8571428571429"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.1479591836735"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="22.280612244898"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="21.5714285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="24" style="0" width="16.7142857142857"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="11.4183673469388"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="14.6224489795918"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.9642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="11.4183673469388"/>
+    <col min="1" max="1" width="8.5703125"/>
+    <col min="2" max="2" width="11.42578125"/>
+    <col min="3" max="3" width="15"/>
+    <col min="4" max="4" width="10.28515625"/>
+    <col min="5" max="5" width="8.5703125"/>
+    <col min="6" max="6" width="6"/>
+    <col min="7" max="7" width="14"/>
+    <col min="8" max="8" width="9.5703125"/>
+    <col min="9" max="9" width="17.42578125"/>
+    <col min="10" max="10" width="17.28515625"/>
+    <col min="11" max="11" width="11.140625"/>
+    <col min="12" max="12" width="11.28515625"/>
+    <col min="13" max="13" width="8.28515625"/>
+    <col min="14" max="14" width="10.7109375"/>
+    <col min="15" max="15" width="15.85546875"/>
+    <col min="16" max="16" width="17.5703125"/>
+    <col min="17" max="17" width="9.7109375"/>
+    <col min="18" max="18" width="15.85546875"/>
+    <col min="19" max="19" width="18.42578125"/>
+    <col min="20" max="20" width="15.85546875"/>
+    <col min="21" max="21" width="15.140625"/>
+    <col min="22" max="22" width="22.28515625"/>
+    <col min="23" max="23" width="21.5703125"/>
+    <col min="25" max="25" width="24.42578125" customWidth="1"/>
+    <col min="26" max="26" width="11" customWidth="1"/>
+    <col min="27" max="28" width="16.7109375"/>
+    <col min="29" max="29" width="11.42578125"/>
+    <col min="30" max="30" width="14.5703125"/>
+    <col min="31" max="31" width="16"/>
+    <col min="32" max="1028" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:31" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,22 +1054,31 @@
         <v>22</v>
       </c>
       <c r="X1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -799,7 +1087,7 @@
       <c r="D2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="6" t="n">
+      <c r="E2" s="6">
         <v>11</v>
       </c>
       <c r="F2" s="6"/>
@@ -824,7 +1112,7 @@
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
-      <c r="T2" s="7" t="n">
+      <c r="T2" s="7">
         <v>37653</v>
       </c>
       <c r="U2" s="6" t="s">
@@ -834,8 +1122,11 @@
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>35</v>
       </c>
@@ -844,7 +1135,7 @@
       <c r="D3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="6">
         <v>12</v>
       </c>
       <c r="F3" s="8"/>
@@ -869,7 +1160,7 @@
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
-      <c r="T3" s="7" t="n">
+      <c r="T3" s="7">
         <v>37654</v>
       </c>
       <c r="U3" s="6" t="s">
@@ -879,8 +1170,11 @@
       <c r="W3" s="8"/>
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>42</v>
       </c>
@@ -889,7 +1183,7 @@
       <c r="D4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="E4" s="6">
         <v>13</v>
       </c>
       <c r="F4" s="8"/>
@@ -914,7 +1208,7 @@
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="7" t="n">
+      <c r="T4" s="7">
         <v>37655</v>
       </c>
       <c r="U4" s="6" t="s">
@@ -924,8 +1218,11 @@
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>49</v>
       </c>
@@ -934,7 +1231,7 @@
       <c r="D5" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="6">
         <v>14</v>
       </c>
       <c r="F5" s="8"/>
@@ -959,7 +1256,7 @@
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
-      <c r="T5" s="7" t="n">
+      <c r="T5" s="7">
         <v>37656</v>
       </c>
       <c r="U5" s="6" t="s">
@@ -969,8 +1266,11 @@
       <c r="W5" s="8"/>
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>56</v>
       </c>
@@ -979,7 +1279,7 @@
       <c r="D6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="6" t="n">
+      <c r="E6" s="6">
         <v>15</v>
       </c>
       <c r="F6" s="8"/>
@@ -1004,7 +1304,7 @@
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
-      <c r="T6" s="7" t="n">
+      <c r="T6" s="7">
         <v>37657</v>
       </c>
       <c r="U6" s="6" t="s">
@@ -1014,8 +1314,11 @@
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>63</v>
       </c>
@@ -1024,7 +1327,7 @@
       <c r="D7" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="6">
         <v>16</v>
       </c>
       <c r="F7" s="9"/>
@@ -1049,7 +1352,7 @@
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
-      <c r="T7" s="7" t="n">
+      <c r="T7" s="7">
         <v>37658</v>
       </c>
       <c r="U7" s="6" t="s">
@@ -1059,15 +1362,18 @@
       <c r="W7" s="9"/>
       <c r="X7" s="9"/>
       <c r="Y7" s="9"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="6" t="n">
+      <c r="E8" s="6">
         <v>17</v>
       </c>
       <c r="F8" s="8"/>
@@ -1092,7 +1398,7 @@
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
-      <c r="T8" s="7" t="n">
+      <c r="T8" s="7">
         <v>37659</v>
       </c>
       <c r="U8" s="6" t="s">
@@ -1102,8 +1408,11 @@
       <c r="W8" s="8"/>
       <c r="X8" s="8"/>
       <c r="Y8" s="8"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>76</v>
       </c>
@@ -1112,7 +1421,7 @@
       <c r="D9" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E9" s="6">
         <v>18</v>
       </c>
       <c r="F9" s="8"/>
@@ -1137,7 +1446,7 @@
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
-      <c r="T9" s="7" t="n">
+      <c r="T9" s="7">
         <v>37660</v>
       </c>
       <c r="U9" s="6" t="s">
@@ -1147,46 +1456,41 @@
       <c r="W9" s="8"/>
       <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.85714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.1428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7040816326531"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="20.9948979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.2908163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.2908163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.8571428571429"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.7142857142857"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="20.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.4183673469388"/>
+    <col min="1" max="1" width="7.85546875"/>
+    <col min="2" max="2" width="16.5703125"/>
+    <col min="3" max="3" width="13.5703125"/>
+    <col min="4" max="4" width="11.140625"/>
+    <col min="5" max="5" width="13.7109375"/>
+    <col min="6" max="7" width="21"/>
+    <col min="8" max="8" width="16.28515625"/>
+    <col min="9" max="9" width="25.28515625"/>
+    <col min="10" max="10" width="14.85546875"/>
+    <col min="11" max="11" width="23.7109375"/>
+    <col min="12" max="13" width="20.7109375"/>
+    <col min="14" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1224,7 +1528,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>28</v>
       </c>
@@ -1233,11 +1537,11 @@
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
-      <c r="E2" s="8" t="n">
+      <c r="E2" s="8">
         <v>11</v>
       </c>
-      <c r="F2" s="11" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="F2" s="11" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="G2" s="11"/>
@@ -1251,7 +1555,7 @@
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>35</v>
       </c>
@@ -1260,10 +1564,10 @@
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
-      <c r="E3" s="8" t="n">
+      <c r="E3" s="8">
         <v>12</v>
       </c>
-      <c r="F3" s="11" t="n">
+      <c r="F3" s="11">
         <v>0</v>
       </c>
       <c r="G3" s="11"/>
@@ -1277,7 +1581,7 @@
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>42</v>
       </c>
@@ -1286,7 +1590,7 @@
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="8" t="n">
+      <c r="E4" s="8">
         <v>13</v>
       </c>
       <c r="F4" s="11" t="s">
@@ -1303,7 +1607,7 @@
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>49</v>
       </c>
@@ -1312,7 +1616,7 @@
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="8" t="n">
+      <c r="E5" s="8">
         <v>14</v>
       </c>
       <c r="F5" s="11"/>
@@ -1327,7 +1631,7 @@
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>56</v>
       </c>
@@ -1336,7 +1640,7 @@
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="8" t="n">
+      <c r="E6" s="8">
         <v>15</v>
       </c>
       <c r="F6" s="11"/>
@@ -1351,7 +1655,7 @@
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>63</v>
       </c>
@@ -1360,7 +1664,7 @@
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="8" t="n">
+      <c r="E7" s="8">
         <v>16</v>
       </c>
       <c r="F7" s="11"/>
@@ -1375,14 +1679,14 @@
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8" t="s">
         <v>113</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="8" t="n">
+      <c r="E8" s="8">
         <v>17</v>
       </c>
       <c r="F8" s="11"/>
@@ -1397,7 +1701,7 @@
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>76</v>
       </c>
@@ -1406,7 +1710,7 @@
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="8" t="n">
+      <c r="E9" s="8">
         <v>18</v>
       </c>
       <c r="F9" s="11"/>
@@ -1422,39 +1726,31 @@
       <c r="L9" s="11"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.8571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.7142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.4183673469388"/>
+    <col min="1" max="1" width="11.42578125"/>
+    <col min="2" max="2" width="16.85546875"/>
+    <col min="3" max="3" width="13.85546875"/>
+    <col min="4" max="4" width="13.5703125"/>
+    <col min="5" max="5" width="17.28515625"/>
+    <col min="6" max="6" width="23.7109375"/>
+    <col min="7" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1474,7 +1770,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>28</v>
       </c>
@@ -1490,7 +1786,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>35</v>
       </c>
@@ -1506,7 +1802,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>42</v>
       </c>
@@ -1522,7 +1818,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>49</v>
       </c>
@@ -1538,7 +1834,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>56</v>
       </c>
@@ -1554,7 +1850,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>63</v>
       </c>
@@ -1570,7 +1866,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11" t="s">
         <v>113</v>
@@ -1584,7 +1880,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>76</v>
       </c>
@@ -1601,42 +1897,34 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.85714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.8571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.7091836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.7091836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.4234693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.4183673469388"/>
+    <col min="1" max="1" width="7.85546875"/>
+    <col min="2" max="2" width="16.85546875"/>
+    <col min="3" max="3" width="13.85546875"/>
+    <col min="4" max="4" width="14.85546875"/>
+    <col min="5" max="5" width="18.5703125"/>
+    <col min="6" max="6" width="21.7109375"/>
+    <col min="7" max="7" width="26.7109375"/>
+    <col min="8" max="8" width="26.42578125"/>
+    <col min="9" max="9" width="24.5703125"/>
+    <col min="10" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1665,7 +1953,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>28</v>
       </c>
@@ -1688,7 +1976,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>35</v>
       </c>
@@ -1711,7 +1999,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>42</v>
       </c>
@@ -1734,7 +2022,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>49</v>
       </c>
@@ -1757,7 +2045,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>56</v>
       </c>
@@ -1780,7 +2068,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>63</v>
       </c>
@@ -1803,7 +2091,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11" t="s">
         <v>113</v>
@@ -1824,7 +2112,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>76</v>
       </c>
@@ -1848,12 +2136,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[TM-47] Added automatable in test case import and export
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/import-columns.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/import-columns.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace_squashtm\squashtest-tm-staging\tm\tm.service\src\test\resources\batchimport\testcase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaceSquashTM\squashtest-tm-staging\tm\tm.service\src\test\resources\batchimport\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BE10F5-0F4F-4678-BEFD-886A16A2528C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEST_CASES" sheetId="1" r:id="rId1"/>
@@ -17,12 +18,20 @@
     <sheet name="PARAMETERS" sheetId="3" r:id="rId3"/>
     <sheet name="DATASETS" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="156">
   <si>
     <t>ACTION</t>
   </si>
@@ -487,12 +496,15 @@
   </si>
   <si>
     <t>TC_SCRIPT</t>
+  </si>
+  <si>
+    <t>TC_AUTOMATABLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -518,7 +530,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -612,11 +624,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -629,12 +652,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{0B8F6EC6-974C-4AC3-8444-BB2BB2C4A8A9}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -942,11 +994,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AF9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA11" sqref="AA11"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,20 +1022,20 @@
     <col min="17" max="17" width="9.7109375"/>
     <col min="18" max="18" width="15.85546875"/>
     <col min="19" max="19" width="18.42578125"/>
-    <col min="20" max="20" width="15.85546875"/>
-    <col min="21" max="21" width="15.140625"/>
-    <col min="22" max="22" width="22.28515625"/>
-    <col min="23" max="23" width="21.5703125"/>
-    <col min="25" max="25" width="24.42578125" customWidth="1"/>
-    <col min="26" max="26" width="11" customWidth="1"/>
-    <col min="27" max="28" width="16.7109375"/>
-    <col min="29" max="29" width="11.42578125"/>
-    <col min="30" max="30" width="14.5703125"/>
-    <col min="31" max="31" width="16"/>
-    <col min="32" max="1028" width="11.42578125"/>
+    <col min="21" max="21" width="15.85546875"/>
+    <col min="22" max="22" width="15.140625"/>
+    <col min="23" max="23" width="22.28515625"/>
+    <col min="24" max="24" width="21.5703125"/>
+    <col min="26" max="26" width="24.42578125" customWidth="1"/>
+    <col min="27" max="27" width="11" customWidth="1"/>
+    <col min="28" max="29" width="16.7109375"/>
+    <col min="30" max="30" width="11.42578125"/>
+    <col min="31" max="31" width="14.5703125"/>
+    <col min="32" max="32" width="16"/>
+    <col min="33" max="1029" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1042,43 +1094,46 @@
         <v>18</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -1112,21 +1167,22 @@
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
-      <c r="T2" s="7">
+      <c r="T2" s="6"/>
+      <c r="U2" s="7">
         <v>37653</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="V2" s="6"/>
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AC2" s="6"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>35</v>
       </c>
@@ -1160,21 +1216,22 @@
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
-      <c r="T3" s="7">
+      <c r="T3" s="6"/>
+      <c r="U3" s="7">
         <v>37654</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="V3" s="8"/>
       <c r="W3" s="8"/>
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AC3" s="8"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>42</v>
       </c>
@@ -1208,21 +1265,22 @@
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="7">
+      <c r="T4" s="6"/>
+      <c r="U4" s="7">
         <v>37655</v>
       </c>
-      <c r="U4" s="6" t="s">
+      <c r="V4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="8"/>
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
       <c r="AA4" s="8"/>
       <c r="AB4" s="8"/>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AC4" s="8"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>49</v>
       </c>
@@ -1256,21 +1314,22 @@
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
-      <c r="T5" s="7">
+      <c r="T5" s="6"/>
+      <c r="U5" s="7">
         <v>37656</v>
       </c>
-      <c r="U5" s="6" t="s">
+      <c r="V5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="V5" s="8"/>
       <c r="W5" s="8"/>
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
       <c r="Z5" s="8"/>
       <c r="AA5" s="8"/>
       <c r="AB5" s="8"/>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AC5" s="8"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>56</v>
       </c>
@@ -1304,21 +1363,22 @@
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
-      <c r="T6" s="7">
+      <c r="T6" s="6"/>
+      <c r="U6" s="7">
         <v>37657</v>
       </c>
-      <c r="U6" s="6" t="s">
+      <c r="V6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="V6" s="8"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8"/>
       <c r="AB6" s="8"/>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AC6" s="8"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>63</v>
       </c>
@@ -1352,21 +1412,22 @@
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
-      <c r="T7" s="7">
+      <c r="T7" s="12"/>
+      <c r="U7" s="7">
         <v>37658</v>
       </c>
-      <c r="U7" s="6" t="s">
+      <c r="V7" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="V7" s="9"/>
       <c r="W7" s="9"/>
       <c r="X7" s="9"/>
       <c r="Y7" s="9"/>
       <c r="Z7" s="9"/>
       <c r="AA7" s="9"/>
       <c r="AB7" s="9"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AC7" s="9"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1398,21 +1459,22 @@
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
-      <c r="T8" s="7">
+      <c r="T8" s="6"/>
+      <c r="U8" s="7">
         <v>37659</v>
       </c>
-      <c r="U8" s="6" t="s">
+      <c r="V8" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="V8" s="8"/>
       <c r="W8" s="8"/>
       <c r="X8" s="8"/>
       <c r="Y8" s="8"/>
       <c r="Z8" s="8"/>
       <c r="AA8" s="8"/>
       <c r="AB8" s="8"/>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AC8" s="8"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>76</v>
       </c>
@@ -1446,19 +1508,20 @@
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
-      <c r="T9" s="7">
+      <c r="T9" s="6"/>
+      <c r="U9" s="7">
         <v>37660</v>
       </c>
-      <c r="U9" s="6" t="s">
+      <c r="V9" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="V9" s="8"/>
       <c r="W9" s="8"/>
       <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
       <c r="Z9" s="8"/>
       <c r="AA9" s="8"/>
       <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1467,7 +1530,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1732,7 +1795,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1903,7 +1966,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
[TM-13] Excel Test Cases Export deals with UUID
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/import-columns.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/import-columns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaceSquashTM\squashtest-tm-staging\tm\tm.service\src\test\resources\batchimport\testcase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguilhem\Documents\squashtest-tm-staging-clone\tm\tm.service\src\test\resources\batchimport\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BE10F5-0F4F-4678-BEFD-886A16A2528C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB760828-CCD3-4AD4-8224-5156E800F172}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="987" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEST_CASES" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="157">
   <si>
     <t>ACTION</t>
   </si>
@@ -499,6 +499,9 @@
   </si>
   <si>
     <t>TC_AUTOMATABLE</t>
+  </si>
+  <si>
+    <t>TC_UUID</t>
   </si>
 </sst>
 </file>
@@ -995,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF9"/>
+  <dimension ref="A1:AG9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,33 +1012,33 @@
     <col min="4" max="4" width="10.28515625"/>
     <col min="5" max="5" width="8.5703125"/>
     <col min="6" max="6" width="6"/>
-    <col min="7" max="7" width="14"/>
-    <col min="8" max="8" width="9.5703125"/>
-    <col min="9" max="9" width="17.42578125"/>
-    <col min="10" max="10" width="17.28515625"/>
-    <col min="11" max="11" width="11.140625"/>
-    <col min="12" max="12" width="11.28515625"/>
-    <col min="13" max="13" width="8.28515625"/>
-    <col min="14" max="14" width="10.7109375"/>
-    <col min="15" max="15" width="15.85546875"/>
-    <col min="16" max="16" width="17.5703125"/>
-    <col min="17" max="17" width="9.7109375"/>
-    <col min="18" max="18" width="15.85546875"/>
-    <col min="19" max="19" width="18.42578125"/>
-    <col min="21" max="21" width="15.85546875"/>
-    <col min="22" max="22" width="15.140625"/>
-    <col min="23" max="23" width="22.28515625"/>
-    <col min="24" max="24" width="21.5703125"/>
-    <col min="26" max="26" width="24.42578125" customWidth="1"/>
-    <col min="27" max="27" width="11" customWidth="1"/>
-    <col min="28" max="29" width="16.7109375"/>
-    <col min="30" max="30" width="11.42578125"/>
-    <col min="31" max="31" width="14.5703125"/>
-    <col min="32" max="32" width="16"/>
-    <col min="33" max="1029" width="11.42578125"/>
+    <col min="8" max="8" width="14"/>
+    <col min="9" max="9" width="9.5703125"/>
+    <col min="10" max="10" width="17.42578125"/>
+    <col min="11" max="11" width="17.28515625"/>
+    <col min="12" max="12" width="11.140625"/>
+    <col min="13" max="13" width="11.28515625"/>
+    <col min="14" max="14" width="8.28515625"/>
+    <col min="15" max="15" width="10.7109375"/>
+    <col min="16" max="16" width="15.85546875"/>
+    <col min="17" max="17" width="17.5703125"/>
+    <col min="18" max="18" width="9.7109375"/>
+    <col min="19" max="19" width="15.85546875"/>
+    <col min="20" max="20" width="18.42578125"/>
+    <col min="22" max="22" width="15.85546875"/>
+    <col min="23" max="23" width="15.140625"/>
+    <col min="24" max="24" width="22.28515625"/>
+    <col min="25" max="25" width="21.5703125"/>
+    <col min="27" max="27" width="24.42578125" customWidth="1"/>
+    <col min="28" max="28" width="11" customWidth="1"/>
+    <col min="29" max="30" width="16.7109375"/>
+    <col min="31" max="31" width="11.42578125"/>
+    <col min="32" max="32" width="14.5703125"/>
+    <col min="33" max="33" width="16"/>
+    <col min="34" max="1030" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1055,85 +1058,88 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -1146,43 +1152,44 @@
         <v>11</v>
       </c>
       <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="6"/>
+      <c r="P2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
-      <c r="U2" s="7">
+      <c r="U2" s="6"/>
+      <c r="V2" s="7">
         <v>37653</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="W2" s="6"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
       <c r="AC2" s="6"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AD2" s="6"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>35</v>
       </c>
@@ -1195,43 +1202,44 @@
         <v>12</v>
       </c>
       <c r="F3" s="8"/>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="8"/>
+      <c r="H3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="8"/>
+      <c r="P3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="7">
+      <c r="T3" s="8"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="7">
         <v>37654</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="W3" s="8"/>
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
       <c r="AC3" s="8"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AD3" s="8"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>42</v>
       </c>
@@ -1244,43 +1252,44 @@
         <v>13</v>
       </c>
       <c r="F4" s="8"/>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="6"/>
+      <c r="H4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="8"/>
+      <c r="J4" s="6"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="8"/>
+      <c r="P4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="Q4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="7">
+      <c r="T4" s="8"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="7">
         <v>37655</v>
       </c>
-      <c r="V4" s="6" t="s">
+      <c r="W4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="W4" s="8"/>
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
       <c r="AA4" s="8"/>
       <c r="AB4" s="8"/>
       <c r="AC4" s="8"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AD4" s="8"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>49</v>
       </c>
@@ -1293,43 +1302,44 @@
         <v>14</v>
       </c>
       <c r="F5" s="8"/>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
-      <c r="O5" s="6" t="s">
+      <c r="O5" s="8"/>
+      <c r="P5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="Q5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="7">
+      <c r="T5" s="8"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="7">
         <v>37656</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="W5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="W5" s="8"/>
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
       <c r="Z5" s="8"/>
       <c r="AA5" s="8"/>
       <c r="AB5" s="8"/>
       <c r="AC5" s="8"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AD5" s="8"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>56</v>
       </c>
@@ -1342,43 +1352,44 @@
         <v>15</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="8"/>
+      <c r="J6" s="6"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
-      <c r="O6" s="6" t="s">
+      <c r="O6" s="8"/>
+      <c r="P6" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="Q6" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="7">
+      <c r="T6" s="8"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="7">
         <v>37657</v>
       </c>
-      <c r="V6" s="6" t="s">
+      <c r="W6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="W6" s="8"/>
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8"/>
       <c r="AB6" s="8"/>
       <c r="AC6" s="8"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AD6" s="8"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>63</v>
       </c>
@@ -1391,43 +1402,44 @@
         <v>16</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="I7" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
-      <c r="O7" s="6" t="s">
+      <c r="O7" s="9"/>
+      <c r="P7" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="P7" s="6" t="s">
+      <c r="Q7" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="7">
+      <c r="T7" s="9"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="7">
         <v>37658</v>
       </c>
-      <c r="V7" s="6" t="s">
+      <c r="W7" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="W7" s="9"/>
       <c r="X7" s="9"/>
       <c r="Y7" s="9"/>
       <c r="Z7" s="9"/>
       <c r="AA7" s="9"/>
       <c r="AB7" s="9"/>
       <c r="AC7" s="9"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AD7" s="9"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1438,43 +1450,44 @@
         <v>17</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="8"/>
+      <c r="J8" s="6"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="6" t="s">
+      <c r="O8" s="8"/>
+      <c r="P8" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="P8" s="6" t="s">
+      <c r="Q8" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="7">
+      <c r="T8" s="8"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="7">
         <v>37659</v>
       </c>
-      <c r="V8" s="6" t="s">
+      <c r="W8" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="W8" s="8"/>
       <c r="X8" s="8"/>
       <c r="Y8" s="8"/>
       <c r="Z8" s="8"/>
       <c r="AA8" s="8"/>
       <c r="AB8" s="8"/>
       <c r="AC8" s="8"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AD8" s="8"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>76</v>
       </c>
@@ -1487,41 +1500,42 @@
         <v>18</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="8"/>
+      <c r="H9" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="I9" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
-      <c r="O9" s="6" t="s">
+      <c r="O9" s="8"/>
+      <c r="P9" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="P9" s="6" t="s">
+      <c r="Q9" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="7">
+      <c r="T9" s="8"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="7">
         <v>37660</v>
       </c>
-      <c r="V9" s="6" t="s">
+      <c r="W9" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="W9" s="8"/>
       <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
       <c r="Z9" s="8"/>
       <c r="AA9" s="8"/>
       <c r="AB9" s="8"/>
       <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>